<commit_message>
Conexão com banco e criação da entidade funci
</commit_message>
<xml_diff>
--- a/PlanilhaHorasEstagio_Alessandro.xlsx
+++ b/PlanilhaHorasEstagio_Alessandro.xlsx
@@ -24,36 +24,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
-  <si>
-    <t>22:30 - 00:30</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>pesquisa sobre linguagens e como desenvolver uma ecommerce</t>
   </si>
   <si>
-    <t>18:30 - 22:30</t>
-  </si>
-  <si>
     <t>desenvolvimento em  spring boot, com persistência de dados em h2 e utilização de template bootstrap</t>
   </si>
   <si>
-    <t>07:30 - 12:30</t>
-  </si>
-  <si>
     <t xml:space="preserve">Foi feita a analise do processo de desenvolvimento e reiniciado o trabalho por não ter sido considerado o padrão MVC- Plano de ação tomado-- reiniciar projeto Spring boot padrão de desenvolvimento MVC com dependências de JPA, MYSQL, devTools, springWeb, </t>
   </si>
   <si>
-    <t>22:30 - 02:30</t>
-  </si>
-  <si>
     <t>Criado projeto, iniciado a contrução com importação de template, criado repositorio no github, pload de arquivos</t>
+  </si>
+  <si>
+    <t>DATA</t>
+  </si>
+  <si>
+    <t>HORA INICIO</t>
+  </si>
+  <si>
+    <t>HORA TÉRMINO</t>
+  </si>
+  <si>
+    <t>DESCRIÇÃO ATIVIDADES</t>
+  </si>
+  <si>
+    <t>Conectando com o banco de dados e criando relação de persistência com JPA</t>
+  </si>
+  <si>
+    <t>Criando novas entidades como logica de negócio</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="h:mm:ss;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -83,12 +92,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -369,117 +379,210 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:J7"/>
+  <dimension ref="A2:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C10" activeCellId="1" sqref="B10 C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
-    <col min="10" max="10" width="33.7109375" customWidth="1"/>
+    <col min="1" max="2" width="20.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="11" max="11" width="33.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44714</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3">
+        <v>0.9375</v>
+      </c>
+      <c r="C3" s="3">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3" s="2"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44715</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3">
+        <v>0.9375</v>
+      </c>
+      <c r="C4" s="3">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4" s="2"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>44715</v>
       </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="2"/>
+      <c r="B5" s="3">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.9375</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5" s="2"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>44716</v>
       </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="2"/>
+      <c r="B6" s="3">
+        <v>0.3125</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44721</v>
       </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="2"/>
+      <c r="B7" s="3">
+        <v>0.9375</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>44723</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.3125</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>44724</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C9" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>44731</v>
+      </c>
+      <c r="B10" s="3">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="C10" s="3">
+        <v>5.9027777777777783E-2</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="C6:J6"/>
-    <mergeCell ref="C7:J7"/>
+  <mergeCells count="8">
+    <mergeCell ref="D8:K8"/>
+    <mergeCell ref="D9:K9"/>
+    <mergeCell ref="D2:K2"/>
+    <mergeCell ref="D3:K3"/>
+    <mergeCell ref="D4:K4"/>
+    <mergeCell ref="D5:K5"/>
+    <mergeCell ref="D6:K6"/>
+    <mergeCell ref="D7:K7"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>